<commit_message>
student dashboard and general update
- student dashboard completed
- updated data source.py with the common variables that will use across the dashboard
- updated notebook
</commit_message>
<xml_diff>
--- a/Student Survey - July.xlsx
+++ b/Student Survey - July.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveswinburneeduau-my.sharepoint.com/personal/104436984_student_swin_edu_au/Documents/2023 S2/COS60011/Wk1/git/Swin-TDP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="11_C25CCE5B2A8756483D92D6B398011B1F7D1BAE8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B9D1879-4CF0-4D4C-B7B8-CA100366F76F}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="11_C25CCE5B2A8756483D92D6B398011B1F7D1BAE8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D3A27E0-6C98-463C-88D6-9F49071F4CA8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_dictionary!$A$1:$G$44</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">net_0_Friends!$A$1:$B$1258</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">net_2_Feedback!$A$1:$B$241</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">net_3_MoreTime!$A$1:$B$481</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">net_affiliation_0_SchoolActivit!$A$1:$C$416</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">responses!$M$1:$M$175</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">responses!$A$1:$AK$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -16663,8 +16665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K175"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22816,7 +22818,7 @@
   <dimension ref="A1:AK175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42601,7 +42603,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="M1:M175" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <autoFilter ref="A1:AK1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -42611,8 +42613,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:B1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1266" sqref="G1266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42745,7 +42747,7 @@
         <v>38003</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>37915</v>
       </c>
@@ -42753,7 +42755,7 @@
         <v>37941</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <v>37915</v>
       </c>
@@ -42761,7 +42763,7 @@
         <v>37929</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>37915</v>
       </c>
@@ -42769,7 +42771,7 @@
         <v>37934</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="34">
         <v>37915</v>
       </c>
@@ -42777,7 +42779,7 @@
         <v>37948</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>37915</v>
       </c>
@@ -43057,7 +43059,7 @@
         <v>37854</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="34">
         <v>38009</v>
       </c>
@@ -43065,7 +43067,7 @@
         <v>37952</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="35">
         <v>38009</v>
       </c>
@@ -43073,7 +43075,7 @@
         <v>37912</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="34">
         <v>38009</v>
       </c>
@@ -43081,7 +43083,7 @@
         <v>37953</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="35">
         <v>38009</v>
       </c>
@@ -43089,7 +43091,7 @@
         <v>37856</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="34">
         <v>38009</v>
       </c>
@@ -52305,7 +52307,7 @@
         <v>37935</v>
       </c>
     </row>
-    <row r="1212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1212" s="34">
         <v>37856</v>
       </c>
@@ -52313,7 +52315,7 @@
         <v>37912</v>
       </c>
     </row>
-    <row r="1213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1213" s="35">
         <v>37856</v>
       </c>
@@ -52321,7 +52323,7 @@
         <v>37958</v>
       </c>
     </row>
-    <row r="1214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1214" s="34">
         <v>37856</v>
       </c>
@@ -52329,7 +52331,7 @@
         <v>37983</v>
       </c>
     </row>
-    <row r="1215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1215" s="35">
         <v>37856</v>
       </c>
@@ -52337,7 +52339,7 @@
         <v>38009</v>
       </c>
     </row>
-    <row r="1216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1216" s="34">
         <v>37856</v>
       </c>
@@ -52345,7 +52347,7 @@
         <v>37953</v>
       </c>
     </row>
-    <row r="1217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1217" s="35">
         <v>37856</v>
       </c>
@@ -52353,7 +52355,7 @@
         <v>37952</v>
       </c>
     </row>
-    <row r="1218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1218" s="34">
         <v>37856</v>
       </c>
@@ -52361,7 +52363,7 @@
         <v>38014</v>
       </c>
     </row>
-    <row r="1219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1219" s="35">
         <v>37856</v>
       </c>
@@ -52685,8 +52687,7 @@
   <autoFilter ref="A1:B1258" xr:uid="{00000000-0001-0000-0500-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="37856"/>
-        <filter val="38009"/>
+        <filter val="37915"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -52699,7 +52700,7 @@
   <dimension ref="A1:F309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55806,11 +55807,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:B241"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43:N45"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -55822,7 +55822,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34">
         <v>37881</v>
       </c>
@@ -55830,7 +55830,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35">
         <v>37881</v>
       </c>
@@ -55838,7 +55838,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
         <v>37980</v>
       </c>
@@ -55846,7 +55846,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35">
         <v>37980</v>
       </c>
@@ -55862,7 +55862,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35">
         <v>37998</v>
       </c>
@@ -55870,7 +55870,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34">
         <v>37998</v>
       </c>
@@ -55878,7 +55878,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="35">
         <v>37998</v>
       </c>
@@ -55886,7 +55886,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
         <v>38007</v>
       </c>
@@ -55894,7 +55894,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="35">
         <v>37982</v>
       </c>
@@ -55902,7 +55902,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34">
         <v>37982</v>
       </c>
@@ -55910,7 +55910,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="35">
         <v>37910</v>
       </c>
@@ -55918,7 +55918,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
         <v>37851</v>
       </c>
@@ -55926,7 +55926,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>37993</v>
       </c>
@@ -55934,7 +55934,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34">
         <v>37880</v>
       </c>
@@ -55942,7 +55942,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>37880</v>
       </c>
@@ -55950,7 +55950,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <v>37880</v>
       </c>
@@ -55958,7 +55958,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>37917</v>
       </c>
@@ -55966,7 +55966,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34">
         <v>37917</v>
       </c>
@@ -55974,7 +55974,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>38008</v>
       </c>
@@ -55982,7 +55982,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34">
         <v>38008</v>
       </c>
@@ -55990,7 +55990,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="35">
         <v>38008</v>
       </c>
@@ -55998,7 +55998,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34">
         <v>37859</v>
       </c>
@@ -56006,7 +56006,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>37876</v>
       </c>
@@ -56014,7 +56014,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="34">
         <v>37876</v>
       </c>
@@ -56022,7 +56022,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
         <v>38011</v>
       </c>
@@ -56030,7 +56030,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34">
         <v>38011</v>
       </c>
@@ -56038,7 +56038,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35">
         <v>38011</v>
       </c>
@@ -56046,7 +56046,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34">
         <v>38011</v>
       </c>
@@ -56054,7 +56054,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="35">
         <v>38016</v>
       </c>
@@ -56062,7 +56062,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="34">
         <v>38016</v>
       </c>
@@ -56070,7 +56070,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35">
         <v>37952</v>
       </c>
@@ -56078,7 +56078,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="34">
         <v>37952</v>
       </c>
@@ -56086,7 +56086,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="35">
         <v>38019</v>
       </c>
@@ -56094,7 +56094,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="34">
         <v>37992</v>
       </c>
@@ -56102,7 +56102,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="35">
         <v>37986</v>
       </c>
@@ -56110,7 +56110,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="34">
         <v>37986</v>
       </c>
@@ -56118,7 +56118,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="35">
         <v>37986</v>
       </c>
@@ -56126,7 +56126,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34">
         <v>37888</v>
       </c>
@@ -56134,7 +56134,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="35">
         <v>37916</v>
       </c>
@@ -56142,7 +56142,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34">
         <v>37916</v>
       </c>
@@ -56150,7 +56150,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="35">
         <v>37916</v>
       </c>
@@ -56158,7 +56158,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="34">
         <v>37999</v>
       </c>
@@ -56166,7 +56166,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="35">
         <v>37867</v>
       </c>
@@ -56174,7 +56174,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="34">
         <v>37891</v>
       </c>
@@ -56182,7 +56182,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="35">
         <v>37891</v>
       </c>
@@ -56190,7 +56190,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="34">
         <v>37853</v>
       </c>
@@ -56198,7 +56198,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="35">
         <v>37945</v>
       </c>
@@ -56206,7 +56206,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="34">
         <v>37878</v>
       </c>
@@ -56214,7 +56214,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="35">
         <v>37878</v>
       </c>
@@ -56222,7 +56222,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="34">
         <v>37878</v>
       </c>
@@ -56230,7 +56230,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="35">
         <v>37955</v>
       </c>
@@ -56238,7 +56238,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="34">
         <v>38003</v>
       </c>
@@ -56246,7 +56246,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="35">
         <v>38003</v>
       </c>
@@ -56254,7 +56254,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="34">
         <v>38003</v>
       </c>
@@ -56262,7 +56262,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="35">
         <v>37918</v>
       </c>
@@ -56270,7 +56270,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="34">
         <v>37906</v>
       </c>
@@ -56278,7 +56278,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="35">
         <v>37906</v>
       </c>
@@ -56286,7 +56286,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="34">
         <v>37936</v>
       </c>
@@ -56294,7 +56294,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="35">
         <v>37936</v>
       </c>
@@ -56302,7 +56302,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="34">
         <v>37855</v>
       </c>
@@ -56310,7 +56310,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="35">
         <v>37855</v>
       </c>
@@ -56318,7 +56318,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="34">
         <v>37855</v>
       </c>
@@ -56326,7 +56326,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="35">
         <v>37855</v>
       </c>
@@ -56334,7 +56334,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="34">
         <v>38001</v>
       </c>
@@ -56342,7 +56342,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="35">
         <v>37921</v>
       </c>
@@ -56350,7 +56350,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="34">
         <v>37921</v>
       </c>
@@ -56358,7 +56358,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="35">
         <v>37921</v>
       </c>
@@ -56366,7 +56366,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="34">
         <v>37857</v>
       </c>
@@ -56374,7 +56374,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="35">
         <v>37857</v>
       </c>
@@ -56382,7 +56382,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="34">
         <v>37904</v>
       </c>
@@ -56390,7 +56390,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="35">
         <v>37904</v>
       </c>
@@ -56398,7 +56398,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="34">
         <v>38006</v>
       </c>
@@ -56406,7 +56406,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="35">
         <v>37894</v>
       </c>
@@ -56414,7 +56414,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="34">
         <v>37894</v>
       </c>
@@ -56422,7 +56422,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="35">
         <v>37965</v>
       </c>
@@ -56430,7 +56430,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="34">
         <v>37995</v>
       </c>
@@ -56438,7 +56438,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="35">
         <v>37971</v>
       </c>
@@ -56446,7 +56446,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="34">
         <v>37971</v>
       </c>
@@ -56454,7 +56454,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="35">
         <v>37971</v>
       </c>
@@ -56462,7 +56462,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="34">
         <v>37971</v>
       </c>
@@ -56470,7 +56470,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="35">
         <v>37971</v>
       </c>
@@ -56478,7 +56478,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="34">
         <v>37971</v>
       </c>
@@ -56486,7 +56486,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="35">
         <v>37971</v>
       </c>
@@ -56494,7 +56494,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="34">
         <v>37985</v>
       </c>
@@ -56502,7 +56502,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="35">
         <v>37985</v>
       </c>
@@ -56510,7 +56510,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="34">
         <v>37985</v>
       </c>
@@ -56518,7 +56518,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="35">
         <v>37985</v>
       </c>
@@ -56526,7 +56526,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="34">
         <v>37985</v>
       </c>
@@ -56534,7 +56534,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="35">
         <v>37985</v>
       </c>
@@ -56542,7 +56542,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="34">
         <v>37914</v>
       </c>
@@ -56550,7 +56550,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="35">
         <v>37914</v>
       </c>
@@ -56558,7 +56558,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="34">
         <v>37933</v>
       </c>
@@ -56566,7 +56566,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="35">
         <v>37988</v>
       </c>
@@ -56574,7 +56574,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="34">
         <v>37862</v>
       </c>
@@ -56582,7 +56582,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="35">
         <v>37951</v>
       </c>
@@ -56590,7 +56590,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="34">
         <v>37951</v>
       </c>
@@ -56598,7 +56598,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="35">
         <v>37951</v>
       </c>
@@ -56606,7 +56606,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="34">
         <v>37950</v>
       </c>
@@ -56614,7 +56614,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="35">
         <v>37950</v>
       </c>
@@ -56622,7 +56622,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="34">
         <v>37929</v>
       </c>
@@ -56630,7 +56630,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="35">
         <v>37964</v>
       </c>
@@ -56638,7 +56638,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="34">
         <v>37964</v>
       </c>
@@ -56646,7 +56646,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="35">
         <v>37947</v>
       </c>
@@ -56654,7 +56654,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="34">
         <v>37947</v>
       </c>
@@ -56662,7 +56662,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="35">
         <v>37947</v>
       </c>
@@ -56670,7 +56670,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="34">
         <v>37870</v>
       </c>
@@ -56678,7 +56678,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="35">
         <v>37912</v>
       </c>
@@ -56686,7 +56686,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="34">
         <v>37889</v>
       </c>
@@ -56694,7 +56694,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="35">
         <v>37889</v>
       </c>
@@ -56702,7 +56702,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="34">
         <v>37889</v>
       </c>
@@ -56710,7 +56710,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="35">
         <v>37858</v>
       </c>
@@ -56718,7 +56718,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="34">
         <v>37858</v>
       </c>
@@ -56726,7 +56726,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="35">
         <v>37858</v>
       </c>
@@ -56734,7 +56734,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="34">
         <v>37927</v>
       </c>
@@ -56742,7 +56742,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="35">
         <v>37927</v>
       </c>
@@ -56750,7 +56750,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="34">
         <v>37960</v>
       </c>
@@ -56758,7 +56758,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="35">
         <v>37887</v>
       </c>
@@ -56766,7 +56766,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="34">
         <v>37854</v>
       </c>
@@ -56774,7 +56774,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="35">
         <v>37854</v>
       </c>
@@ -56782,7 +56782,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="34">
         <v>37852</v>
       </c>
@@ -56790,7 +56790,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="35">
         <v>37932</v>
       </c>
@@ -56798,7 +56798,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="34">
         <v>37932</v>
       </c>
@@ -56806,7 +56806,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="35">
         <v>37907</v>
       </c>
@@ -56814,7 +56814,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="34">
         <v>37907</v>
       </c>
@@ -56822,7 +56822,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="35">
         <v>37996</v>
       </c>
@@ -56830,7 +56830,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="34">
         <v>37996</v>
       </c>
@@ -56838,7 +56838,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="35">
         <v>37970</v>
       </c>
@@ -56846,7 +56846,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="34">
         <v>37970</v>
       </c>
@@ -56854,7 +56854,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="35">
         <v>37970</v>
       </c>
@@ -56862,7 +56862,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="34">
         <v>37885</v>
       </c>
@@ -56870,7 +56870,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="35">
         <v>37885</v>
       </c>
@@ -56878,7 +56878,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="34">
         <v>37885</v>
       </c>
@@ -56886,7 +56886,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="35">
         <v>37983</v>
       </c>
@@ -56894,7 +56894,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="34">
         <v>37983</v>
       </c>
@@ -56902,7 +56902,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="35">
         <v>37983</v>
       </c>
@@ -56910,7 +56910,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="34">
         <v>37939</v>
       </c>
@@ -56918,7 +56918,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="35">
         <v>37939</v>
       </c>
@@ -56926,7 +56926,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="34">
         <v>37978</v>
       </c>
@@ -56934,7 +56934,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="35">
         <v>37966</v>
       </c>
@@ -56942,7 +56942,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="34">
         <v>37966</v>
       </c>
@@ -56950,7 +56950,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="35">
         <v>37944</v>
       </c>
@@ -56958,7 +56958,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="34">
         <v>37884</v>
       </c>
@@ -56966,7 +56966,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="35">
         <v>37953</v>
       </c>
@@ -56974,7 +56974,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="34">
         <v>38000</v>
       </c>
@@ -56982,7 +56982,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="35">
         <v>38015</v>
       </c>
@@ -56990,7 +56990,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="34">
         <v>37977</v>
       </c>
@@ -56998,7 +56998,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="35">
         <v>37977</v>
       </c>
@@ -57006,7 +57006,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="34">
         <v>37961</v>
       </c>
@@ -57014,7 +57014,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="35">
         <v>37961</v>
       </c>
@@ -57022,7 +57022,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="34">
         <v>37962</v>
       </c>
@@ -57030,7 +57030,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="35">
         <v>37974</v>
       </c>
@@ -57038,7 +57038,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="34">
         <v>37974</v>
       </c>
@@ -57046,7 +57046,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="35">
         <v>37974</v>
       </c>
@@ -57054,7 +57054,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="34">
         <v>37974</v>
       </c>
@@ -57062,7 +57062,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="35">
         <v>37896</v>
       </c>
@@ -57070,7 +57070,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="34">
         <v>37896</v>
       </c>
@@ -57078,7 +57078,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="35">
         <v>37873</v>
       </c>
@@ -57086,7 +57086,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="34">
         <v>37873</v>
       </c>
@@ -57094,7 +57094,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="35">
         <v>37905</v>
       </c>
@@ -57102,7 +57102,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="34">
         <v>37895</v>
       </c>
@@ -57110,7 +57110,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="35">
         <v>37895</v>
       </c>
@@ -57118,7 +57118,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="34">
         <v>37895</v>
       </c>
@@ -57126,7 +57126,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="35">
         <v>37976</v>
       </c>
@@ -57134,7 +57134,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="34">
         <v>37989</v>
       </c>
@@ -57142,7 +57142,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="35">
         <v>37989</v>
       </c>
@@ -57150,7 +57150,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="34">
         <v>37989</v>
       </c>
@@ -57158,7 +57158,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="35">
         <v>37860</v>
       </c>
@@ -57166,7 +57166,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="34">
         <v>37860</v>
       </c>
@@ -57174,7 +57174,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="35">
         <v>38022</v>
       </c>
@@ -57182,7 +57182,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="34">
         <v>37920</v>
       </c>
@@ -57190,7 +57190,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="35">
         <v>37920</v>
       </c>
@@ -57198,7 +57198,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="34">
         <v>37908</v>
       </c>
@@ -57206,7 +57206,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="35">
         <v>38014</v>
       </c>
@@ -57214,7 +57214,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="34">
         <v>37872</v>
       </c>
@@ -57222,7 +57222,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="35">
         <v>37959</v>
       </c>
@@ -57230,7 +57230,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="34">
         <v>37959</v>
       </c>
@@ -57238,7 +57238,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="35">
         <v>37959</v>
       </c>
@@ -57246,7 +57246,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="34">
         <v>37967</v>
       </c>
@@ -57254,7 +57254,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="35">
         <v>37967</v>
       </c>
@@ -57262,7 +57262,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="34">
         <v>37967</v>
       </c>
@@ -57270,7 +57270,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="35">
         <v>37969</v>
       </c>
@@ -57278,7 +57278,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="34">
         <v>37969</v>
       </c>
@@ -57286,7 +57286,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="35">
         <v>37963</v>
       </c>
@@ -57294,7 +57294,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="34">
         <v>37963</v>
       </c>
@@ -57302,7 +57302,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="35">
         <v>37963</v>
       </c>
@@ -57310,7 +57310,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="34">
         <v>37963</v>
       </c>
@@ -57318,7 +57318,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="35">
         <v>37850</v>
       </c>
@@ -57326,7 +57326,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="34">
         <v>37850</v>
       </c>
@@ -57334,7 +57334,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="35">
         <v>38013</v>
       </c>
@@ -57342,7 +57342,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="34">
         <v>38013</v>
       </c>
@@ -57350,7 +57350,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="35">
         <v>37913</v>
       </c>
@@ -57358,7 +57358,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="34">
         <v>37913</v>
       </c>
@@ -57366,7 +57366,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="35">
         <v>37913</v>
       </c>
@@ -57374,7 +57374,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="34">
         <v>37990</v>
       </c>
@@ -57382,7 +57382,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="35">
         <v>37990</v>
       </c>
@@ -57390,7 +57390,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="34">
         <v>37990</v>
       </c>
@@ -57398,7 +57398,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="35">
         <v>37877</v>
       </c>
@@ -57406,7 +57406,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="34">
         <v>37877</v>
       </c>
@@ -57414,7 +57414,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="35">
         <v>38012</v>
       </c>
@@ -57422,7 +57422,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="34">
         <v>38012</v>
       </c>
@@ -57430,7 +57430,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="35">
         <v>37868</v>
       </c>
@@ -57438,7 +57438,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="34">
         <v>37868</v>
       </c>
@@ -57446,7 +57446,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="35">
         <v>37886</v>
       </c>
@@ -57454,7 +57454,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="34">
         <v>37886</v>
       </c>
@@ -57462,7 +57462,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="35">
         <v>37954</v>
       </c>
@@ -57470,7 +57470,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="34">
         <v>37981</v>
       </c>
@@ -57478,7 +57478,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="35">
         <v>37981</v>
       </c>
@@ -57486,7 +57486,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="34">
         <v>37981</v>
       </c>
@@ -57494,7 +57494,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="35">
         <v>37981</v>
       </c>
@@ -57502,7 +57502,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="34">
         <v>37997</v>
       </c>
@@ -57510,7 +57510,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="35">
         <v>37924</v>
       </c>
@@ -57518,7 +57518,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="34">
         <v>37903</v>
       </c>
@@ -57526,7 +57526,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="35">
         <v>37903</v>
       </c>
@@ -57534,7 +57534,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="34">
         <v>37994</v>
       </c>
@@ -57542,7 +57542,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="35">
         <v>37994</v>
       </c>
@@ -57550,7 +57550,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="34">
         <v>37946</v>
       </c>
@@ -57558,7 +57558,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="35">
         <v>37946</v>
       </c>
@@ -57566,7 +57566,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="34">
         <v>37901</v>
       </c>
@@ -57574,7 +57574,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="35">
         <v>37948</v>
       </c>
@@ -57582,7 +57582,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="34">
         <v>37973</v>
       </c>
@@ -57590,7 +57590,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="35">
         <v>37973</v>
       </c>
@@ -57598,7 +57598,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="34">
         <v>37866</v>
       </c>
@@ -57606,7 +57606,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="35">
         <v>37866</v>
       </c>
@@ -57614,7 +57614,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="34">
         <v>37919</v>
       </c>
@@ -57622,7 +57622,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="35">
         <v>37919</v>
       </c>
@@ -57630,7 +57630,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="34">
         <v>37938</v>
       </c>
@@ -57638,7 +57638,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="35">
         <v>37938</v>
       </c>
@@ -57646,7 +57646,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="34">
         <v>37941</v>
       </c>
@@ -57654,7 +57654,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="35">
         <v>37984</v>
       </c>
@@ -57662,7 +57662,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="34">
         <v>37984</v>
       </c>
@@ -57670,7 +57670,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="35">
         <v>37975</v>
       </c>
@@ -57678,7 +57678,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="34">
         <v>37892</v>
       </c>
@@ -57686,7 +57686,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="35">
         <v>37892</v>
       </c>
@@ -57694,7 +57694,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="34">
         <v>37928</v>
       </c>
@@ -57702,7 +57702,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="35">
         <v>37928</v>
       </c>
@@ -57710,7 +57710,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="34">
         <v>38021</v>
       </c>
@@ -57718,7 +57718,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="35">
         <v>38021</v>
       </c>
@@ -57726,7 +57726,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="34">
         <v>37902</v>
       </c>
@@ -57734,7 +57734,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="35">
         <v>37902</v>
       </c>
@@ -57743,6 +57743,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B241" xr:uid="{00000000-0001-0000-0700-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="37915"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -57752,7 +57759,7 @@
   <dimension ref="A1:B481"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61606,6 +61613,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B481" xr:uid="{00000000-0001-0000-0800-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>